<commit_message>
Server to Local on 09 02 24
</commit_message>
<xml_diff>
--- a/public/Generated/report.xlsx
+++ b/public/Generated/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Submitted Date</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Section1</t>
   </si>
   <si>
-    <t>Section2</t>
-  </si>
-  <si>
     <t>Secured Marks</t>
   </si>
   <si>
@@ -37,7 +34,52 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Lokesh Akurathi</t>
+    <t>Bhakata Ram Suna</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Not Cleared</t>
+  </si>
+  <si>
+    <t>Auto Submitted Assessment (Moved Outside the assessment boundary).</t>
+  </si>
+  <si>
+    <t>Swati Swarupa Rajguru</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Sanigdha Mohanty</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Satyajeet behera</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Switching of Tab's detected.</t>
+  </si>
+  <si>
+    <t>Smitaranjan Samantaray</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Soumyaranjan Sethy</t>
   </si>
   <si>
     <t>100</t>
@@ -46,7 +88,28 @@
     <t>Cleared</t>
   </si>
   <si>
-    <t>Switching of Tab's detected.</t>
+    <t>Jagadish Prasad Dash</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>Gagan Kumar Behura</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Time Out Auto Submitting the Assessment.</t>
+  </si>
+  <si>
+    <t>Kollu Nagarjuna</t>
+  </si>
+  <si>
+    <t>65</t>
   </si>
 </sst>
 </file>
@@ -424,18 +487,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="4" width="10" customWidth="1"/>
-    <col min="5" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,25 +520,22 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>45258.282905092594</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -483,8 +543,235 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>63</v>
+      </c>
+      <c r="D5">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>61</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>57</v>
+      </c>
+      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45330.49493055556</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>